<commit_message>
organize code and files
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,41 +468,248 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Chris Bierfreund</t>
+          <t>Alexander Götz von olenhusen</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>167</v>
+        <v>49</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>jersey dark man M (34€), jersey light man M (34€), jersey_long black man M (38€), short multisport S (22€), hoodie_zip man M (49€)</t>
+          <t>hoodie_zip man L (49€)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Annika Nolte</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>49</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>hoodie_zip woman M (49€)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Chris Bierfreund</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>167</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>jersey dark man M (34€), jersey light man M (34€), jersey_long black man M (38€), short multisport S (22€), hoodie_zip man M (49€)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Elena Gugganig</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>80</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>jersey dark woman L (34€), jersey light woman L (34€), short woman M (22€)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Hannes Drobek</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>109</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>jersey_long black man L (38€), tank dark man L (29€), hoodie_no_zip man L (42€)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ingo Schmiegel</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>209</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>jersey dark man L (34€), jersey light man L (34€), jersey_long black man L (38€), short multisport L (22€), hoodie_no_zip man L (42€), hoodie_zip man L (49€)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Julia Busse</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>tank light woman L (29€), short multisport L (22€), hoodie_zip woman M (49€)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Katharina Wilbrandt</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>22</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>short multisport XL (22€)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Matthis Heimberg</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>109</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>jersey_long black man L (38€), tank dark man L (29€), hoodie_no_zip man L (42€)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>Nils Hoffmann</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C11" t="n">
         <v>80</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D11" t="n">
         <v>1</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>jersey dark man S (34€), jersey light man S (34€), short multisport M (22€)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Patrick Jung</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>80</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>jersey dark man L (34€), jersey light man L (34€), short long L (22€)</t>
         </is>
       </c>
     </row>

</xml_diff>